<commit_message>
Ajuste no caminho do arquivo Excel
</commit_message>
<xml_diff>
--- a/static/excel/ASEXCEL2021.xlsx
+++ b/static/excel/ASEXCEL2021.xlsx
@@ -12737,16 +12737,16 @@
     <row r="2">
       <c r="A2" s="123" t="inlineStr">
         <is>
-          <t>0012/2021</t>
+          <t>0015/2021</t>
         </is>
       </c>
       <c r="B2" s="123" t="inlineStr">
         <is>
-          <t>7210.2020/0001136-3</t>
+          <t>7210.2020/0001900-3</t>
         </is>
       </c>
       <c r="C2" s="122" t="n">
-        <v>44441</v>
+        <v>44400</v>
       </c>
       <c r="D2" s="123" t="inlineStr">
         <is>
@@ -12765,7 +12765,7 @@
       </c>
       <c r="G2" s="123" t="inlineStr">
         <is>
-          <t>Recon Produtora e Eventos Eireli</t>
+          <t>Desintec - Serviços Técnicos Ltda - EPP</t>
         </is>
       </c>
       <c r="H2" s="123" t="inlineStr">

</xml_diff>